<commit_message>
Add 2019 F1040 Schedules 2 and 3
</commit_message>
<xml_diff>
--- a/Federal/f1040s2-2019.xlsx
+++ b/Federal/f1040s2-2019.xlsx
@@ -205,18 +205,18 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -515,14 +515,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -530,54 +530,54 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <f>SUM(F4:F5)</f>
         <v>0</v>
       </c>
@@ -588,124 +588,124 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="4" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="4" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="4" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="10"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="4" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <f>SUM(F9:F14)</f>
         <v>0</v>
       </c>
@@ -717,6 +717,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B16:D16"/>
@@ -725,11 +730,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>